<commit_message>
pushed by me the project which i have done
</commit_message>
<xml_diff>
--- a/SDET9/testData/Excel.xlsx
+++ b/SDET9/testData/Excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{95574BB5-ECCA-4AF6-B987-58AD7B8011D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{98D24466-D478-4EF0-9C7F-13EC1BA393E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="14460" windowHeight="12300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="14490" windowHeight="12300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>url</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>sony</t>
+  </si>
+  <si>
+    <t>productName</t>
+  </si>
+  <si>
+    <t>Bisleri</t>
   </si>
 </sst>
 </file>
@@ -459,10 +465,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A79CBD97-FF38-4574-98DE-9E44DC95AE29}">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A2:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,6 +484,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>